<commit_message>
Moved functions to gaopaw module, improved analysis workflow
</commit_message>
<xml_diff>
--- a/Results/Accuracy.xlsx
+++ b/Results/Accuracy.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>GAOPAW</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Se</t>
+  </si>
+  <si>
+    <t>Br</t>
   </si>
   <si>
     <t>Rb</t>
@@ -1271,7 +1274,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="5">
-        <v>185.206</v>
+        <v>39.515</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1916,13 +1919,23 @@
       <c r="Z51" s="2"/>
     </row>
     <row r="52">
-      <c r="B52" s="5"/>
+      <c r="B52" s="5">
+        <v>1.225</v>
+      </c>
       <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+      <c r="D52" s="5">
+        <v>2.572</v>
+      </c>
+      <c r="E52" s="5">
+        <v>1.247</v>
+      </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="5"/>
+      <c r="G52" s="5">
+        <v>2.572</v>
+      </c>
+      <c r="H52" s="5">
+        <v>51.763</v>
+      </c>
       <c r="I52" s="4"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -2000,13 +2013,23 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
+      <c r="B55" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C55" s="5">
+        <v>0.378</v>
+      </c>
+      <c r="D55" s="5">
+        <v>0.878</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0.331</v>
+      </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="5"/>
+      <c r="H55" s="5">
+        <v>31.295</v>
+      </c>
       <c r="I55" s="4"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -2084,13 +2107,23 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58">
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
+      <c r="B58" s="5">
+        <v>0.484</v>
+      </c>
+      <c r="C58" s="5">
+        <v>0.55</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0.851</v>
+      </c>
+      <c r="E58" s="5">
+        <v>10.696</v>
+      </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
-      <c r="H58" s="5"/>
+      <c r="H58" s="5">
+        <v>48.62</v>
+      </c>
       <c r="I58" s="4"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -2168,13 +2201,23 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61">
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
+      <c r="B61" s="5">
+        <v>1.202</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0.826</v>
+      </c>
+      <c r="D61" s="5">
+        <v>0.805</v>
+      </c>
+      <c r="E61" s="5">
+        <v>1.926</v>
+      </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
-      <c r="H61" s="5"/>
+      <c r="H61" s="5">
+        <v>188.083</v>
+      </c>
       <c r="I61" s="4"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -2252,13 +2295,23 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64">
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
+      <c r="B64" s="5">
+        <v>0.739</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1.074</v>
+      </c>
+      <c r="D64" s="5">
+        <v>0.682</v>
+      </c>
+      <c r="E64" s="5">
+        <v>16.256</v>
+      </c>
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
-      <c r="H64" s="5"/>
+      <c r="H64" s="5">
+        <v>50.402</v>
+      </c>
       <c r="I64" s="4"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -2336,13 +2389,23 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67">
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="4"/>
+      <c r="B67" s="5">
+        <v>0.075</v>
+      </c>
+      <c r="C67" s="5">
+        <v>1.019</v>
+      </c>
+      <c r="D67" s="5">
+        <v>0.593</v>
+      </c>
       <c r="E67" s="4"/>
-      <c r="F67" s="5"/>
+      <c r="F67" s="5">
+        <v>3.093</v>
+      </c>
       <c r="G67" s="4"/>
-      <c r="H67" s="5"/>
+      <c r="H67" s="5">
+        <v>21.178</v>
+      </c>
       <c r="I67" s="4"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -2420,13 +2483,23 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70">
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="4"/>
+      <c r="B70" s="5">
+        <v>0.057</v>
+      </c>
+      <c r="C70" s="5">
+        <v>1.059</v>
+      </c>
+      <c r="D70" s="5">
+        <v>3.197</v>
+      </c>
       <c r="E70" s="4"/>
-      <c r="F70" s="5"/>
+      <c r="F70" s="5">
+        <v>0.783</v>
+      </c>
       <c r="G70" s="4"/>
-      <c r="H70" s="5"/>
+      <c r="H70" s="5">
+        <v>17.404</v>
+      </c>
       <c r="I70" s="4"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -2504,13 +2577,23 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73">
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="4"/>
+      <c r="B73" s="5">
+        <v>0.619</v>
+      </c>
+      <c r="C73" s="5">
+        <v>1.1</v>
+      </c>
+      <c r="D73" s="5">
+        <v>0.19</v>
+      </c>
       <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="F73" s="5">
+        <v>0.522</v>
+      </c>
       <c r="G73" s="4"/>
-      <c r="H73" s="5"/>
+      <c r="H73" s="5">
+        <v>30.866</v>
+      </c>
       <c r="I73" s="4"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -2588,13 +2671,23 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76">
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="4"/>
+      <c r="B76" s="5">
+        <v>1.279</v>
+      </c>
+      <c r="C76" s="5">
+        <v>1.044</v>
+      </c>
+      <c r="D76" s="5">
+        <v>0.444</v>
+      </c>
       <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
+      <c r="F76" s="5">
+        <v>9.267</v>
+      </c>
       <c r="G76" s="4"/>
-      <c r="H76" s="5"/>
+      <c r="H76" s="5">
+        <v>51.264</v>
+      </c>
       <c r="I76" s="4"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -2672,13 +2765,23 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79">
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="4"/>
+      <c r="B79" s="5">
+        <v>0.337</v>
+      </c>
+      <c r="C79" s="5">
+        <v>0.447</v>
+      </c>
+      <c r="D79" s="5">
+        <v>0.253</v>
+      </c>
       <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
+      <c r="F79" s="5">
+        <v>43.407</v>
+      </c>
       <c r="G79" s="4"/>
-      <c r="H79" s="5"/>
+      <c r="H79" s="5">
+        <v>75.484</v>
+      </c>
       <c r="I79" s="4"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -2756,13 +2859,23 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82">
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
+      <c r="B82" s="5">
+        <v>0.559</v>
+      </c>
+      <c r="C82" s="5">
+        <v>0.322</v>
+      </c>
+      <c r="D82" s="5">
+        <v>0.736</v>
+      </c>
+      <c r="E82" s="5">
+        <v>4.162</v>
+      </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
-      <c r="H82" s="5"/>
+      <c r="H82" s="5">
+        <v>29.457</v>
+      </c>
       <c r="I82" s="4"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -2840,13 +2953,23 @@
       <c r="Z84" s="2"/>
     </row>
     <row r="85">
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
+      <c r="B85" s="5">
+        <v>0.318</v>
+      </c>
+      <c r="C85" s="5">
+        <v>0.814</v>
+      </c>
+      <c r="D85" s="5">
+        <v>0.383</v>
+      </c>
+      <c r="E85" s="5">
+        <v>0.884</v>
+      </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
-      <c r="H85" s="5"/>
+      <c r="H85" s="5">
+        <v>22.414</v>
+      </c>
       <c r="I85" s="4"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -2924,13 +3047,23 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88">
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
+      <c r="B88" s="3">
+        <v>0.289</v>
+      </c>
+      <c r="C88" s="3">
+        <v>0.458</v>
+      </c>
+      <c r="D88" s="3">
+        <v>0.468</v>
+      </c>
+      <c r="E88" s="3">
+        <v>4.788</v>
+      </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="3"/>
+      <c r="H88" s="3">
+        <v>39.163</v>
+      </c>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
@@ -3008,13 +3141,23 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91">
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
+      <c r="B91" s="3">
+        <v>0.177</v>
+      </c>
+      <c r="C91" s="3">
+        <v>0.348</v>
+      </c>
+      <c r="D91" s="3">
+        <v>0.839</v>
+      </c>
+      <c r="E91" s="3">
+        <v>5.018</v>
+      </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="3"/>
+      <c r="H91" s="3">
+        <v>625.908</v>
+      </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -3092,13 +3235,23 @@
       <c r="Z93" s="2"/>
     </row>
     <row r="94">
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
+      <c r="B94" s="3">
+        <v>0.653</v>
+      </c>
+      <c r="C94" s="3">
+        <v>0.458</v>
+      </c>
+      <c r="D94" s="3">
+        <v>0.265</v>
+      </c>
+      <c r="E94" s="3">
+        <v>40.79</v>
+      </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="3"/>
+      <c r="H94" s="3">
+        <v>31.46</v>
+      </c>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
@@ -3176,13 +3329,23 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97">
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
+      <c r="B97" s="3">
+        <v>0.412</v>
+      </c>
+      <c r="C97" s="3">
+        <v>0.299</v>
+      </c>
+      <c r="D97" s="3">
+        <v>0.153</v>
+      </c>
+      <c r="E97" s="3">
+        <v>0.834</v>
+      </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="3"/>
+      <c r="H97" s="3">
+        <v>52.54</v>
+      </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -3231,7 +3394,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3260,13 +3423,23 @@
       <c r="Z99" s="2"/>
     </row>
     <row r="100">
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
+      <c r="B100" s="3">
+        <v>0.391</v>
+      </c>
+      <c r="C100" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="D100" s="3">
+        <v>0.755</v>
+      </c>
+      <c r="E100" s="3">
+        <v>15.531</v>
+      </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="3"/>
+      <c r="H100" s="3">
+        <v>125.613</v>
+      </c>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -3315,7 +3488,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3399,7 +3572,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3483,7 +3656,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3567,7 +3740,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3651,7 +3824,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3735,7 +3908,7 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3819,7 +3992,7 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3903,7 +4076,7 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3987,7 +4160,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -4071,7 +4244,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4155,7 +4328,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4239,7 +4412,7 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4323,7 +4496,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4407,7 +4580,7 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -4491,7 +4664,7 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -4575,7 +4748,7 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -4659,7 +4832,7 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -4743,7 +4916,7 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -4827,7 +5000,7 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -4911,7 +5084,7 @@
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -4995,7 +5168,7 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -5079,7 +5252,7 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -5163,7 +5336,7 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -5247,7 +5420,7 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -5331,7 +5504,7 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -5415,7 +5588,7 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -5499,7 +5672,7 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -5583,7 +5756,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -5667,7 +5840,7 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -5751,7 +5924,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -5835,7 +6008,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -5919,7 +6092,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -6003,7 +6176,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>

</xml_diff>

<commit_message>
Added script to automate variable writing in dakota.in, work in progress
</commit_message>
<xml_diff>
--- a/Results/Accuracy.xlsx
+++ b/Results/Accuracy.xlsx
@@ -34,7 +34,7 @@
     <t>Phonons (THz)</t>
   </si>
   <si>
-    <t>Band gap (%)</t>
+    <t>Band gap (eV)</t>
   </si>
   <si>
     <t>Magnetization (%)</t>
@@ -515,7 +515,7 @@
         <v>1.707</v>
       </c>
       <c r="E7" s="5">
-        <v>0.359</v>
+        <v>0.05</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5">
@@ -611,7 +611,7 @@
         <v>0.45</v>
       </c>
       <c r="E10" s="5">
-        <v>0.579</v>
+        <v>0.033</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -705,7 +705,7 @@
         <v>0.825</v>
       </c>
       <c r="E13" s="5">
-        <v>0.307</v>
+        <v>0.026</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -799,7 +799,7 @@
         <v>1.989</v>
       </c>
       <c r="E16" s="5">
-        <v>2.207</v>
+        <v>0.1</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -893,7 +893,7 @@
         <v>0.617</v>
       </c>
       <c r="E19" s="5">
-        <v>11.411</v>
+        <v>0.14</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -987,7 +987,7 @@
         <v>0.983</v>
       </c>
       <c r="E22" s="5">
-        <v>1.343</v>
+        <v>0.01</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1081,7 +1081,7 @@
         <v>1.473</v>
       </c>
       <c r="E25" s="5">
-        <v>1.171</v>
+        <v>0.055</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1175,7 +1175,7 @@
         <v>0.465</v>
       </c>
       <c r="E28" s="5">
-        <v>2.572</v>
+        <v>0.18</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1269,7 +1269,7 @@
         <v>1.282</v>
       </c>
       <c r="E31" s="5">
-        <v>0.382</v>
+        <v>0.02</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1363,7 +1363,7 @@
         <v>1.473</v>
       </c>
       <c r="E34" s="3">
-        <v>1.171</v>
+        <v>0.05</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1457,7 +1457,7 @@
         <v>0.15</v>
       </c>
       <c r="E37" s="3">
-        <v>1.591</v>
+        <v>0.07</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="3">
@@ -1553,7 +1553,7 @@
         <v>0.376</v>
       </c>
       <c r="E40" s="5">
-        <v>9.513</v>
+        <v>0.105</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1647,7 +1647,7 @@
         <v>0.363</v>
       </c>
       <c r="E43" s="5">
-        <v>1.739</v>
+        <v>0.03</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1741,7 +1741,7 @@
         <v>0.272</v>
       </c>
       <c r="E46" s="5">
-        <v>0.566</v>
+        <v>0.015</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1835,7 +1835,7 @@
         <v>1.537</v>
       </c>
       <c r="E49" s="5">
-        <v>0.382</v>
+        <v>0.02</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1927,7 +1927,7 @@
         <v>2.572</v>
       </c>
       <c r="E52" s="5">
-        <v>1.247</v>
+        <v>0.09</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="5">
@@ -2023,7 +2023,7 @@
         <v>0.878</v>
       </c>
       <c r="E55" s="5">
-        <v>0.331</v>
+        <v>0.008</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -2117,7 +2117,7 @@
         <v>0.851</v>
       </c>
       <c r="E58" s="5">
-        <v>10.696</v>
+        <v>0.15</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2211,7 +2211,7 @@
         <v>0.805</v>
       </c>
       <c r="E61" s="5">
-        <v>1.926</v>
+        <v>0.038</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -2305,7 +2305,7 @@
         <v>0.682</v>
       </c>
       <c r="E64" s="5">
-        <v>16.256</v>
+        <v>0.281</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
@@ -2869,7 +2869,7 @@
         <v>0.736</v>
       </c>
       <c r="E82" s="5">
-        <v>4.162</v>
+        <v>0.045</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -2963,7 +2963,7 @@
         <v>0.383</v>
       </c>
       <c r="E85" s="5">
-        <v>0.884</v>
+        <v>0.018</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
@@ -3057,7 +3057,7 @@
         <v>0.468</v>
       </c>
       <c r="E88" s="3">
-        <v>4.788</v>
+        <v>0.073</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -3151,7 +3151,7 @@
         <v>0.839</v>
       </c>
       <c r="E91" s="3">
-        <v>5.018</v>
+        <v>0.002</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3245,7 +3245,7 @@
         <v>0.265</v>
       </c>
       <c r="E94" s="3">
-        <v>40.79</v>
+        <v>0.125</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3339,7 +3339,7 @@
         <v>0.153</v>
       </c>
       <c r="E97" s="3">
-        <v>0.834</v>
+        <v>0.019</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -3433,7 +3433,7 @@
         <v>0.755</v>
       </c>
       <c r="E100" s="3">
-        <v>15.531</v>
+        <v>0.252</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -28660,15 +28660,49 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="A189:A191"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A168:A170"/>
+    <mergeCell ref="A165:A167"/>
+    <mergeCell ref="A162:A164"/>
+    <mergeCell ref="A171:A173"/>
+    <mergeCell ref="A174:A176"/>
+    <mergeCell ref="A120:A122"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="A126:A128"/>
+    <mergeCell ref="A135:A137"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="A147:A149"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="A180:A182"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="A195:A197"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="A177:A179"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
     <mergeCell ref="A105:A107"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
     <mergeCell ref="A108:A110"/>
     <mergeCell ref="A84:A86"/>
     <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A48:A50"/>
     <mergeCell ref="A51:A53"/>
     <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
@@ -28676,56 +28710,22 @@
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B3:H4"/>
+    <mergeCell ref="A27:A29"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B3:H4"/>
     <mergeCell ref="A93:A95"/>
     <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="A120:A122"/>
     <mergeCell ref="A111:A113"/>
     <mergeCell ref="A114:A116"/>
     <mergeCell ref="A78:A80"/>
     <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="A180:A182"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="A192:A194"/>
-    <mergeCell ref="A195:A197"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="A189:A191"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A168:A170"/>
-    <mergeCell ref="A165:A167"/>
-    <mergeCell ref="A162:A164"/>
-    <mergeCell ref="A171:A173"/>
-    <mergeCell ref="A174:A176"/>
-    <mergeCell ref="A177:A179"/>
+    <mergeCell ref="A57:A59"/>
     <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="A147:A149"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A126:A128"/>
-    <mergeCell ref="A135:A137"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="A150:A152"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="A156:A158"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>